<commit_message>
Fixed errors regarding data formatting not being applied to categories other than TRA.
</commit_message>
<xml_diff>
--- a/data/Grouped_Competitors_by_Discipline.xlsx
+++ b/data/Grouped_Competitors_by_Discipline.xlsx
@@ -16,177 +16,177 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="80">
   <si>
     <t>#</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Club</t>
+  </si>
+  <si>
+    <t>Antwerp Flazgod</t>
+  </si>
+  <si>
+    <t>DCU</t>
+  </si>
+  <si>
+    <t>Derbiled Áed</t>
+  </si>
+  <si>
+    <t>Karpos Pankratios</t>
+  </si>
+  <si>
+    <t>QUB</t>
+  </si>
+  <si>
+    <t>Yolotzin Thibaut</t>
+  </si>
+  <si>
+    <t>UCC</t>
+  </si>
+  <si>
+    <t>Sören Shiva</t>
+  </si>
+  <si>
+    <t>TCD</t>
+  </si>
+  <si>
+    <t>Brianne Hagano</t>
+  </si>
+  <si>
+    <t>UL</t>
+  </si>
+  <si>
+    <t>Aäron Óscar</t>
+  </si>
+  <si>
+    <t>UCD</t>
+  </si>
+  <si>
+    <t>Désirée Godofredo</t>
+  </si>
+  <si>
+    <t>Bjoern Pierrick</t>
+  </si>
+  <si>
+    <t>Shoshanna Assol</t>
+  </si>
+  <si>
+    <t>Akma 2</t>
+  </si>
+  <si>
+    <t>Echo Longray</t>
+  </si>
+  <si>
+    <t>Exeter</t>
+  </si>
+  <si>
+    <t>TEst11</t>
+  </si>
+  <si>
+    <t>Lirana Willowshade</t>
+  </si>
+  <si>
+    <t>Anwar Fateh</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>TEst23</t>
+  </si>
+  <si>
+    <t>Test10</t>
+  </si>
+  <si>
+    <t>Test12</t>
+  </si>
+  <si>
+    <t>Test13</t>
+  </si>
+  <si>
+    <t>Test14</t>
+  </si>
+  <si>
+    <t>Test15</t>
+  </si>
+  <si>
+    <t>Flight 2</t>
+  </si>
+  <si>
+    <t>Test16</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>Test4</t>
+  </si>
+  <si>
+    <t>Test17</t>
+  </si>
+  <si>
+    <t>Test5</t>
+  </si>
+  <si>
+    <t>Test18</t>
+  </si>
+  <si>
+    <t>Test6</t>
+  </si>
+  <si>
+    <t>Test19</t>
+  </si>
+  <si>
+    <t>Test7</t>
+  </si>
+  <si>
+    <t>Test8</t>
+  </si>
+  <si>
+    <t>Test20</t>
+  </si>
+  <si>
+    <t>Test9</t>
+  </si>
+  <si>
+    <t>Test21</t>
+  </si>
+  <si>
+    <t>Test22</t>
+  </si>
+  <si>
+    <t>Test24</t>
+  </si>
+  <si>
+    <t>Test25</t>
+  </si>
+  <si>
+    <t>Flight 3</t>
+  </si>
+  <si>
+    <t>Test26</t>
+  </si>
+  <si>
+    <t>Test27</t>
+  </si>
+  <si>
+    <t>TRAMPOLINE INDIVIDUAL COMPETITORS</t>
+  </si>
+  <si>
+    <t>Novice Men +</t>
+  </si>
+  <si>
     <t>Flight 1</t>
-  </si>
-  <si>
-    <t>Flight 2</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Antwerp Flazgod</t>
-  </si>
-  <si>
-    <t>Anwar Fateh</t>
-  </si>
-  <si>
-    <t>TEst11</t>
-  </si>
-  <si>
-    <t>Test1</t>
-  </si>
-  <si>
-    <t>Test10</t>
-  </si>
-  <si>
-    <t>Test12</t>
-  </si>
-  <si>
-    <t>Test13</t>
-  </si>
-  <si>
-    <t>Test14</t>
-  </si>
-  <si>
-    <t>Test15</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>Test3</t>
-  </si>
-  <si>
-    <t>Test4</t>
-  </si>
-  <si>
-    <t>Test5</t>
-  </si>
-  <si>
-    <t>Test6</t>
-  </si>
-  <si>
-    <t>Test7</t>
-  </si>
-  <si>
-    <t>Test8</t>
-  </si>
-  <si>
-    <t>Test9</t>
-  </si>
-  <si>
-    <t>Club</t>
-  </si>
-  <si>
-    <t>DCU</t>
-  </si>
-  <si>
-    <t>Exeter</t>
-  </si>
-  <si>
-    <t>MU</t>
-  </si>
-  <si>
-    <t>UCC</t>
-  </si>
-  <si>
-    <t>UCD</t>
-  </si>
-  <si>
-    <t>TCD</t>
-  </si>
-  <si>
-    <t>UL</t>
-  </si>
-  <si>
-    <t>Derbiled Áed</t>
-  </si>
-  <si>
-    <t>Flight 3</t>
-  </si>
-  <si>
-    <t>Karpos Pankratios</t>
-  </si>
-  <si>
-    <t>TEst23</t>
-  </si>
-  <si>
-    <t>Test16</t>
-  </si>
-  <si>
-    <t>Test17</t>
-  </si>
-  <si>
-    <t>Test18</t>
-  </si>
-  <si>
-    <t>Test19</t>
-  </si>
-  <si>
-    <t>Test20</t>
-  </si>
-  <si>
-    <t>Test21</t>
-  </si>
-  <si>
-    <t>Test22</t>
-  </si>
-  <si>
-    <t>Test24</t>
-  </si>
-  <si>
-    <t>Test25</t>
-  </si>
-  <si>
-    <t>Test26</t>
-  </si>
-  <si>
-    <t>Test27</t>
-  </si>
-  <si>
-    <t>QUB</t>
-  </si>
-  <si>
-    <t>Yolotzin Thibaut</t>
-  </si>
-  <si>
-    <t>Sören Shiva</t>
-  </si>
-  <si>
-    <t>Brianne Hagano</t>
-  </si>
-  <si>
-    <t>Lirana Willowshade</t>
-  </si>
-  <si>
-    <t>Aäron Óscar</t>
-  </si>
-  <si>
-    <t>Désirée Godofredo</t>
-  </si>
-  <si>
-    <t>Bjoern Pierrick</t>
-  </si>
-  <si>
-    <t>Shoshanna Assol</t>
-  </si>
-  <si>
-    <t>Akma 2</t>
-  </si>
-  <si>
-    <t>Echo Longray</t>
-  </si>
-  <si>
-    <t>TRAMPOLINE INDIVIDUAL COMPETITORS</t>
-  </si>
-  <si>
-    <t>Novice Men +</t>
   </si>
   <si>
     <t>Novice Ladies +</t>
@@ -820,7 +820,7 @@
   <sheetData>
     <row r="1" spans="2:48">
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -920,7 +920,7 @@
     </row>
     <row r="4" spans="2:48">
       <c r="B4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -985,169 +985,169 @@
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="N5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="R5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="V5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="Z5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="AD5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AF5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="AH5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="AI5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AJ5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="AL5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="AM5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AN5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="AP5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="AQ5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AR5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="AT5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="AU5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AV5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:48">
       <c r="B8" s="2" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="N8" s="2" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="R8" s="2" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="V8" s="2" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Z8" s="2" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AD8" s="2" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="AE8" s="2"/>
       <c r="AF8" s="2"/>
       <c r="AH8" s="2" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="AI8" s="2"/>
       <c r="AJ8" s="2"/>
       <c r="AL8" s="2" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="AM8" s="2"/>
       <c r="AN8" s="2"/>
       <c r="AP8" s="2" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="AQ8" s="2"/>
       <c r="AR8" s="2"/>
       <c r="AT8" s="2" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="AU8" s="2"/>
       <c r="AV8" s="2"/>
@@ -1157,109 +1157,109 @@
         <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="F9" s="4">
         <v>1</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="J9" s="4">
         <v>1</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="N9" s="7">
         <v>1</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="R9" s="7">
         <v>1</v>
       </c>
       <c r="S9" s="8" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="T9" s="9" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="V9" s="4">
         <v>1</v>
       </c>
       <c r="W9" s="5" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="X9" s="6" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="Z9" s="7">
         <v>1</v>
       </c>
       <c r="AA9" s="8" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="AB9" s="9" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="AD9" s="7">
         <v>1</v>
       </c>
       <c r="AE9" s="8" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="AF9" s="9" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="AH9" s="7">
         <v>1</v>
       </c>
       <c r="AI9" s="8" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="AJ9" s="9" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="AL9" s="7">
         <v>1</v>
       </c>
       <c r="AM9" s="8" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="AN9" s="9" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="AP9" s="7">
         <v>1</v>
       </c>
       <c r="AQ9" s="8" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="AR9" s="9" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="AT9" s="7">
         <v>1</v>
       </c>
       <c r="AU9" s="8" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="AV9" s="9" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:48">
@@ -1267,37 +1267,37 @@
         <v>2</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="10">
+        <v>2</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="V10" s="13">
+        <v>2</v>
+      </c>
+      <c r="W10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="10">
-        <v>2</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="10">
-        <v>2</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="V10" s="13">
-        <v>2</v>
-      </c>
-      <c r="W10" s="14" t="s">
-        <v>48</v>
-      </c>
       <c r="X10" s="15" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:48">
@@ -1305,28 +1305,28 @@
         <v>3</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F11" s="10">
         <v>3</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="J11" s="10">
         <v>3</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:48">
@@ -1334,28 +1334,28 @@
         <v>4</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="F12" s="10">
         <v>4</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="J12" s="10">
         <v>4</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:48">
@@ -1363,28 +1363,28 @@
         <v>5</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="F13" s="10">
         <v>5</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="J13" s="10">
         <v>5</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="2:48">
@@ -1392,28 +1392,28 @@
         <v>6</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F14" s="10">
         <v>6</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J14" s="10">
         <v>6</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:48">
@@ -1421,28 +1421,28 @@
         <v>7</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F15" s="10">
         <v>7</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="J15" s="10">
         <v>7</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="L15" s="12" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="2:48">
@@ -1450,28 +1450,28 @@
         <v>8</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F16" s="13">
         <v>8</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="J16" s="10">
         <v>8</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="L16" s="12" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="2:12">
@@ -1479,10 +1479,10 @@
         <v>9</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="14"/>
@@ -1491,10 +1491,10 @@
         <v>9</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:12">
@@ -1502,7 +1502,7 @@
       <c r="C18" s="14"/>
       <c r="D18" s="15"/>
       <c r="F18" s="2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1510,15 +1510,15 @@
         <v>10</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L18" s="15" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="2:12">
       <c r="B19" s="2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1526,10 +1526,10 @@
         <v>9</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="J19" s="13"/>
       <c r="K19" s="14"/>
@@ -1540,22 +1540,22 @@
         <v>10</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="F20" s="10">
         <v>10</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -1565,28 +1565,28 @@
         <v>11</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F21" s="10">
         <v>11</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="J21" s="4">
         <v>11</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="2:12">
@@ -1594,28 +1594,28 @@
         <v>12</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="F22" s="10">
         <v>12</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="J22" s="10">
         <v>12</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="2:12">
@@ -1623,28 +1623,28 @@
         <v>13</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F23" s="10">
         <v>13</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="J23" s="10">
         <v>13</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="L23" s="12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="2:12">
@@ -1652,28 +1652,28 @@
         <v>14</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F24" s="10">
         <v>14</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="J24" s="10">
         <v>14</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="L24" s="12" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="2:12">
@@ -1681,28 +1681,28 @@
         <v>15</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F25" s="10">
         <v>15</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="J25" s="10">
         <v>15</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="L25" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="2:12">
@@ -1710,28 +1710,28 @@
         <v>16</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F26" s="13">
         <v>16</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="J26" s="10">
         <v>16</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="L26" s="12" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="2:12">
@@ -1739,19 +1739,19 @@
         <v>17</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="J27" s="10">
         <v>17</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="L27" s="12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="2:12">
@@ -1759,19 +1759,19 @@
         <v>18</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="J28" s="10">
         <v>18</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="L28" s="12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="2:12">
@@ -1779,10 +1779,10 @@
         <v>19</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="L29" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="2:12">
@@ -1792,7 +1792,7 @@
     </row>
     <row r="31" spans="2:12">
       <c r="J31" s="2" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
@@ -1802,10 +1802,10 @@
         <v>20</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="10:12">
@@ -1813,10 +1813,10 @@
         <v>21</v>
       </c>
       <c r="K33" s="11" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="L33" s="12" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="10:12">
@@ -1824,10 +1824,10 @@
         <v>22</v>
       </c>
       <c r="K34" s="11" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="L34" s="12" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="10:12">
@@ -1835,10 +1835,10 @@
         <v>23</v>
       </c>
       <c r="K35" s="11" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="L35" s="12" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="10:12">
@@ -1846,10 +1846,10 @@
         <v>24</v>
       </c>
       <c r="K36" s="11" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="L36" s="12" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="10:12">
@@ -1857,10 +1857,10 @@
         <v>25</v>
       </c>
       <c r="K37" s="14" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="L37" s="15" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="10:12">
@@ -1868,10 +1868,10 @@
         <v>26</v>
       </c>
       <c r="K38" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="L38" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="10:12">
@@ -1879,10 +1879,10 @@
         <v>27</v>
       </c>
       <c r="K39" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="L39" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="10:12">
@@ -1890,10 +1890,10 @@
         <v>28</v>
       </c>
       <c r="K40" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="L40" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1934,7 +1934,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:X9"/>
+  <dimension ref="B1:X26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2055,142 +2055,338 @@
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="N5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="R5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="V5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="W5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24">
+      <c r="B8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="N8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="R8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="V8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+    </row>
+    <row r="9" spans="2:24">
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="7">
+        <v>1</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" s="7">
+        <v>1</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="R9" s="7">
+        <v>1</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="T9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="V9" s="7">
+        <v>1</v>
+      </c>
+      <c r="W9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="X9" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24">
+      <c r="B10" s="10">
+        <v>2</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24">
+      <c r="B11" s="10">
         <v>3</v>
       </c>
-      <c r="X5" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="2:24">
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>1</v>
-      </c>
-      <c r="N8" t="s">
-        <v>1</v>
-      </c>
-      <c r="R8" t="s">
-        <v>1</v>
-      </c>
-      <c r="V8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:24">
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="C11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24">
+      <c r="B12" s="10">
+        <v>4</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24">
+      <c r="B13" s="10">
+        <v>5</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="D13" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24">
+      <c r="B14" s="10">
+        <v>6</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24">
+      <c r="B15" s="10">
+        <v>7</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:24">
+      <c r="B16" s="13">
+        <v>8</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="4">
+        <v>9</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="10">
+        <v>10</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="10">
+        <v>11</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="10">
+        <v>12</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="13">
+        <v>13</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
         <v>46</v>
       </c>
-      <c r="H9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9" t="s">
-        <v>51</v>
-      </c>
-      <c r="L9" t="s">
-        <v>25</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9" t="s">
-        <v>5</v>
-      </c>
-      <c r="P9" t="s">
-        <v>24</v>
-      </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="S9" t="s">
-        <v>45</v>
-      </c>
-      <c r="T9" t="s">
-        <v>25</v>
-      </c>
-      <c r="V9">
-        <v>1</v>
-      </c>
-      <c r="W9" t="s">
-        <v>31</v>
-      </c>
-      <c r="X9" t="s">
-        <v>44</v>
+      <c r="D26" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="14">
     <mergeCell ref="B1:X2"/>
     <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B18:D18"/>
     <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F8:H8"/>
     <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J8:L8"/>
     <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N8:P8"/>
     <mergeCell ref="R4:T4"/>
+    <mergeCell ref="R8:T8"/>
     <mergeCell ref="V4:X4"/>
+    <mergeCell ref="V8:X8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2198,7 +2394,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:P9"/>
+  <dimension ref="B1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2285,51 +2481,37 @@
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="N5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16">
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>1</v>
-      </c>
-      <c r="N8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:16">
@@ -2337,37 +2519,75 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="L9" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="N9">
         <v>1</v>
       </c>
       <c r="O9" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="P9" t="s">
-        <v>27</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10" t="s">
+        <v>37</v>
+      </c>
+      <c r="P10" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added encoding logic to correct unencoded special characters, wrote up a markdown file going over the different files that are created in order, and quality checked the outputted .csv files.
</commit_message>
<xml_diff>
--- a/data/Grouped_Competitors_by_Discipline.xlsx
+++ b/data/Grouped_Competitors_by_Discipline.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matas\Documents\Academic_WIP\Computer_Science_WIP\Personal\trampoline_competition_scheduler\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52009DC-EC77-4B87-B4AE-9DAF4EE031B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="TRA Flights" sheetId="1" r:id="rId1"/>
@@ -18,12 +12,12 @@
     <sheet name="TUM Flights" sheetId="3" r:id="rId3"/>
     <sheet name="SYN Flights" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="134">
   <si>
     <t>#</t>
   </si>
@@ -430,8 +424,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -577,8 +571,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -586,37 +586,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -654,7 +641,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -688,7 +675,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -723,10 +709,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -899,907 +884,905 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AV17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="1.7265625" customWidth="1"/>
-    <col min="2" max="2" width="4.26953125" customWidth="1"/>
-    <col min="3" max="3" width="17.7265625" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" customWidth="1"/>
-    <col min="5" max="5" width="1.7265625" customWidth="1"/>
-    <col min="6" max="6" width="4.26953125" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="9.7265625" customWidth="1"/>
-    <col min="9" max="9" width="1.7265625" customWidth="1"/>
-    <col min="10" max="10" width="4.26953125" customWidth="1"/>
-    <col min="11" max="11" width="18.7265625" customWidth="1"/>
-    <col min="12" max="12" width="9.7265625" customWidth="1"/>
-    <col min="13" max="13" width="1.7265625" customWidth="1"/>
-    <col min="14" max="14" width="4.26953125" customWidth="1"/>
-    <col min="15" max="15" width="18.7265625" customWidth="1"/>
-    <col min="16" max="16" width="10.7265625" customWidth="1"/>
-    <col min="17" max="17" width="1.7265625" customWidth="1"/>
-    <col min="18" max="18" width="4.26953125" customWidth="1"/>
-    <col min="19" max="19" width="18.7265625" customWidth="1"/>
-    <col min="20" max="20" width="5.7265625" customWidth="1"/>
-    <col min="21" max="21" width="1.7265625" customWidth="1"/>
-    <col min="22" max="22" width="4.26953125" customWidth="1"/>
-    <col min="23" max="23" width="19.7265625" customWidth="1"/>
-    <col min="24" max="24" width="11.7265625" customWidth="1"/>
-    <col min="25" max="25" width="1.7265625" customWidth="1"/>
-    <col min="26" max="26" width="4.26953125" customWidth="1"/>
-    <col min="27" max="27" width="15.7265625" customWidth="1"/>
-    <col min="28" max="28" width="12.7265625" customWidth="1"/>
-    <col min="29" max="29" width="1.7265625" customWidth="1"/>
-    <col min="30" max="30" width="4.26953125" customWidth="1"/>
-    <col min="31" max="31" width="19.7265625" customWidth="1"/>
-    <col min="32" max="32" width="17.7265625" customWidth="1"/>
-    <col min="33" max="33" width="1.7265625" customWidth="1"/>
-    <col min="34" max="34" width="4.26953125" customWidth="1"/>
-    <col min="35" max="35" width="16.7265625" customWidth="1"/>
-    <col min="36" max="36" width="17.7265625" customWidth="1"/>
-    <col min="37" max="37" width="1.7265625" customWidth="1"/>
-    <col min="38" max="38" width="4.26953125" customWidth="1"/>
-    <col min="39" max="39" width="16.7265625" customWidth="1"/>
-    <col min="40" max="40" width="5.7265625" customWidth="1"/>
-    <col min="41" max="41" width="1.7265625" customWidth="1"/>
-    <col min="42" max="42" width="4.26953125" customWidth="1"/>
-    <col min="43" max="43" width="18.7265625" customWidth="1"/>
-    <col min="44" max="44" width="5.7265625" customWidth="1"/>
-    <col min="45" max="45" width="1.7265625" customWidth="1"/>
-    <col min="46" max="46" width="4.26953125" customWidth="1"/>
-    <col min="47" max="47" width="16.7265625" customWidth="1"/>
-    <col min="48" max="48" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="1.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="1.7109375" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="1.7109375" customWidth="1"/>
+    <col min="18" max="18" width="4.28515625" customWidth="1"/>
+    <col min="19" max="19" width="18.7109375" customWidth="1"/>
+    <col min="20" max="20" width="5.7109375" customWidth="1"/>
+    <col min="21" max="21" width="1.7109375" customWidth="1"/>
+    <col min="22" max="22" width="4.28515625" customWidth="1"/>
+    <col min="23" max="23" width="19.7109375" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" customWidth="1"/>
+    <col min="25" max="25" width="1.7109375" customWidth="1"/>
+    <col min="26" max="26" width="4.28515625" customWidth="1"/>
+    <col min="27" max="27" width="15.7109375" customWidth="1"/>
+    <col min="28" max="28" width="12.7109375" customWidth="1"/>
+    <col min="29" max="29" width="1.7109375" customWidth="1"/>
+    <col min="30" max="30" width="4.28515625" customWidth="1"/>
+    <col min="31" max="31" width="19.7109375" customWidth="1"/>
+    <col min="32" max="32" width="17.7109375" customWidth="1"/>
+    <col min="33" max="33" width="1.7109375" customWidth="1"/>
+    <col min="34" max="34" width="4.28515625" customWidth="1"/>
+    <col min="35" max="35" width="16.7109375" customWidth="1"/>
+    <col min="36" max="36" width="17.7109375" customWidth="1"/>
+    <col min="37" max="37" width="1.7109375" customWidth="1"/>
+    <col min="38" max="38" width="4.28515625" customWidth="1"/>
+    <col min="39" max="39" width="16.7109375" customWidth="1"/>
+    <col min="40" max="40" width="5.7109375" customWidth="1"/>
+    <col min="41" max="41" width="1.7109375" customWidth="1"/>
+    <col min="42" max="42" width="4.28515625" customWidth="1"/>
+    <col min="43" max="43" width="18.7109375" customWidth="1"/>
+    <col min="44" max="44" width="5.7109375" customWidth="1"/>
+    <col min="45" max="45" width="1.7109375" customWidth="1"/>
+    <col min="46" max="46" width="4.28515625" customWidth="1"/>
+    <col min="47" max="47" width="16.7109375" customWidth="1"/>
+    <col min="48" max="48" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="2:48">
+      <c r="B1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10"/>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10"/>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10"/>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="10"/>
-      <c r="AV1" s="10"/>
-    </row>
-    <row r="2" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="10"/>
-      <c r="AI2" s="10"/>
-      <c r="AJ2" s="10"/>
-      <c r="AK2" s="10"/>
-      <c r="AL2" s="10"/>
-      <c r="AM2" s="10"/>
-      <c r="AN2" s="10"/>
-      <c r="AO2" s="10"/>
-      <c r="AP2" s="10"/>
-      <c r="AQ2" s="10"/>
-      <c r="AR2" s="10"/>
-      <c r="AS2" s="10"/>
-      <c r="AT2" s="10"/>
-      <c r="AU2" s="10"/>
-      <c r="AV2" s="10"/>
-    </row>
-    <row r="4" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B4" s="11" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1"/>
+      <c r="AV1" s="1"/>
+    </row>
+    <row r="2" spans="2:48">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
+      <c r="AO2" s="1"/>
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1"/>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
+    </row>
+    <row r="4" spans="2:48">
+      <c r="B4" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="F4" s="11" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="F4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="J4" s="11" t="s">
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="J4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="N4" s="11" t="s">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="N4" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="R4" s="11" t="s">
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="R4" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="V4" s="11" t="s">
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="V4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Z4" s="11" t="s">
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Z4" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AA4" s="11"/>
-      <c r="AB4" s="11"/>
-      <c r="AD4" s="11" t="s">
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AD4" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="11"/>
-      <c r="AH4" s="11" t="s">
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AH4" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="AI4" s="11"/>
-      <c r="AJ4" s="11"/>
-      <c r="AL4" s="11" t="s">
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AL4" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="AM4" s="11"/>
-      <c r="AN4" s="11"/>
-      <c r="AP4" s="11" t="s">
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AP4" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AQ4" s="11"/>
-      <c r="AR4" s="11"/>
-      <c r="AT4" s="11" t="s">
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="2"/>
+      <c r="AT4" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="AU4" s="11"/>
-      <c r="AV4" s="11"/>
-    </row>
-    <row r="5" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
+      <c r="AU4" s="2"/>
+      <c r="AV4" s="2"/>
+    </row>
+    <row r="5" spans="2:48">
+      <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="G5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N5" s="1" t="s">
+      <c r="K5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="R5" s="1" t="s">
+      <c r="O5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="S5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="V5" s="1" t="s">
+      <c r="S5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="W5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z5" s="1" t="s">
+      <c r="W5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AA5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AA5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AE5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH5" s="1" t="s">
+      <c r="AE5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AI5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL5" s="1" t="s">
+      <c r="AI5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AM5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AN5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AP5" s="1" t="s">
+      <c r="AM5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AQ5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AR5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT5" s="1" t="s">
+      <c r="AQ5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AU5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AV5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B8" s="11" t="s">
+      <c r="AU5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AV5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:48">
+      <c r="B8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="F8" s="11" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="F8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="J8" s="11" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="J8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="N8" s="11" t="s">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="N8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="R8" s="11" t="s">
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="R8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="V8" s="11" t="s">
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="V8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Z8" s="11" t="s">
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Z8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AA8" s="11"/>
-      <c r="AB8" s="11"/>
-      <c r="AD8" s="11" t="s">
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AD8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="11"/>
-      <c r="AH8" s="11" t="s">
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AH8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AI8" s="11"/>
-      <c r="AJ8" s="11"/>
-      <c r="AL8" s="11" t="s">
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+      <c r="AL8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AM8" s="11"/>
-      <c r="AN8" s="11"/>
-      <c r="AP8" s="11" t="s">
+      <c r="AM8" s="2"/>
+      <c r="AN8" s="2"/>
+      <c r="AP8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AQ8" s="11"/>
-      <c r="AR8" s="11"/>
-      <c r="AT8" s="11" t="s">
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="2"/>
+      <c r="AT8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AU8" s="11"/>
-      <c r="AV8" s="11"/>
-    </row>
-    <row r="9" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="AU8" s="2"/>
+      <c r="AV8" s="2"/>
+    </row>
+    <row r="9" spans="2:48">
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="2">
-        <v>1</v>
-      </c>
-      <c r="K9" s="3" t="s">
+      <c r="J9" s="4">
+        <v>1</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N9" s="2">
-        <v>1</v>
-      </c>
-      <c r="O9" s="3" t="s">
+      <c r="N9" s="4">
+        <v>1</v>
+      </c>
+      <c r="O9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="P9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="R9" s="2">
-        <v>1</v>
-      </c>
-      <c r="S9" s="3" t="s">
+      <c r="R9" s="4">
+        <v>1</v>
+      </c>
+      <c r="S9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="T9" s="4" t="s">
+      <c r="T9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="V9" s="2">
-        <v>1</v>
-      </c>
-      <c r="W9" s="3" t="s">
+      <c r="V9" s="4">
+        <v>1</v>
+      </c>
+      <c r="W9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="X9" s="4" t="s">
+      <c r="X9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="Z9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA9" s="3" t="s">
+      <c r="Z9" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="AB9" s="4" t="s">
+      <c r="AB9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="AD9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE9" s="3" t="s">
+      <c r="AD9" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AF9" s="4" t="s">
+      <c r="AF9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="AH9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI9" s="3" t="s">
+      <c r="AH9" s="4">
+        <v>1</v>
+      </c>
+      <c r="AI9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AJ9" s="4" t="s">
+      <c r="AJ9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AL9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AM9" s="3" t="s">
+      <c r="AL9" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AN9" s="4" t="s">
+      <c r="AN9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="AP9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AQ9" s="3" t="s">
+      <c r="AP9" s="4">
+        <v>1</v>
+      </c>
+      <c r="AQ9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="AR9" s="4" t="s">
+      <c r="AR9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="AT9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AU9" s="3" t="s">
+      <c r="AT9" s="4">
+        <v>1</v>
+      </c>
+      <c r="AU9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AV9" s="4" t="s">
+      <c r="AV9" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B10" s="5">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="10" spans="2:48">
+      <c r="B10" s="7">
+        <v>2</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="5">
-        <v>2</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="F10" s="7">
+        <v>2</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="5">
-        <v>2</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="J10" s="7">
+        <v>2</v>
+      </c>
+      <c r="K10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N10" s="5">
-        <v>2</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="N10" s="7">
+        <v>2</v>
+      </c>
+      <c r="O10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P10" s="6" t="s">
+      <c r="P10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="R10" s="5">
-        <v>2</v>
-      </c>
-      <c r="S10" t="s">
+      <c r="R10" s="7">
+        <v>2</v>
+      </c>
+      <c r="S10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="T10" s="6" t="s">
+      <c r="T10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="V10" s="5">
-        <v>2</v>
-      </c>
-      <c r="W10" t="s">
+      <c r="V10" s="7">
+        <v>2</v>
+      </c>
+      <c r="W10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="X10" s="6" t="s">
+      <c r="X10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="Z10" s="5">
-        <v>2</v>
-      </c>
-      <c r="AA10" t="s">
+      <c r="Z10" s="7">
+        <v>2</v>
+      </c>
+      <c r="AA10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AB10" s="6" t="s">
+      <c r="AB10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AD10" s="5">
-        <v>2</v>
-      </c>
-      <c r="AE10" t="s">
+      <c r="AD10" s="7">
+        <v>2</v>
+      </c>
+      <c r="AE10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AF10" s="6" t="s">
+      <c r="AF10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AH10" s="5">
-        <v>2</v>
-      </c>
-      <c r="AI10" t="s">
+      <c r="AH10" s="7">
+        <v>2</v>
+      </c>
+      <c r="AI10" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AJ10" s="6" t="s">
+      <c r="AJ10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="AL10" s="5">
-        <v>2</v>
-      </c>
-      <c r="AM10" t="s">
+      <c r="AL10" s="7">
+        <v>2</v>
+      </c>
+      <c r="AM10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AN10" s="6" t="s">
+      <c r="AN10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AP10" s="7">
-        <v>2</v>
-      </c>
-      <c r="AQ10" s="8" t="s">
+      <c r="AP10" s="10">
+        <v>2</v>
+      </c>
+      <c r="AQ10" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="AR10" s="9" t="s">
+      <c r="AR10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="AT10" s="5">
-        <v>2</v>
-      </c>
-      <c r="AU10" t="s">
+      <c r="AT10" s="7">
+        <v>2</v>
+      </c>
+      <c r="AU10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AV10" s="6" t="s">
+      <c r="AV10" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B11" s="5">
+    <row r="11" spans="2:48">
+      <c r="B11" s="7">
         <v>3</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="7">
         <v>3</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="7">
         <v>3</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="7">
         <v>3</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O11" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="P11" s="6" t="s">
+      <c r="P11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="R11" s="7">
+      <c r="R11" s="10">
         <v>3</v>
       </c>
-      <c r="S11" s="8" t="s">
+      <c r="S11" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="T11" s="9" t="s">
+      <c r="T11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="V11" s="5">
+      <c r="V11" s="7">
         <v>3</v>
       </c>
-      <c r="W11" t="s">
+      <c r="W11" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="X11" s="6" t="s">
+      <c r="X11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="Z11" s="7">
+      <c r="Z11" s="10">
         <v>3</v>
       </c>
-      <c r="AA11" s="8" t="s">
+      <c r="AA11" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="AB11" s="9" t="s">
+      <c r="AB11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AD11" s="5">
+      <c r="AD11" s="7">
         <v>3</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AE11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AF11" s="6" t="s">
+      <c r="AF11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="AH11" s="5">
+      <c r="AH11" s="7">
         <v>3</v>
       </c>
-      <c r="AI11" t="s">
+      <c r="AI11" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AJ11" s="6" t="s">
+      <c r="AJ11" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="AL11" s="5">
+      <c r="AL11" s="7">
         <v>3</v>
       </c>
-      <c r="AM11" t="s">
+      <c r="AM11" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AN11" s="6" t="s">
+      <c r="AN11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="AT11" s="7">
+      <c r="AT11" s="10">
         <v>3</v>
       </c>
-      <c r="AU11" s="8" t="s">
+      <c r="AU11" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="AV11" s="9" t="s">
+      <c r="AV11" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B12" s="5">
+    <row r="12" spans="2:48">
+      <c r="B12" s="7">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="7">
         <v>4</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="7">
         <v>4</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="L12" s="6" t="s">
+      <c r="L12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="7">
         <v>4</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="P12" s="6" t="s">
+      <c r="P12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="V12" s="5">
+      <c r="V12" s="7">
         <v>4</v>
       </c>
-      <c r="W12" t="s">
+      <c r="W12" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="X12" s="6" t="s">
+      <c r="X12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="AD12" s="7">
+      <c r="AD12" s="10">
         <v>4</v>
       </c>
-      <c r="AE12" s="8" t="s">
+      <c r="AE12" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AF12" s="9" t="s">
+      <c r="AF12" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="AH12" s="5">
+      <c r="AH12" s="7">
         <v>4</v>
       </c>
-      <c r="AI12" t="s">
+      <c r="AI12" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AJ12" s="6" t="s">
+      <c r="AJ12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AL12" s="5">
+      <c r="AL12" s="7">
         <v>4</v>
       </c>
-      <c r="AM12" t="s">
+      <c r="AM12" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AN12" s="6" t="s">
+      <c r="AN12" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B13" s="5">
+    <row r="13" spans="2:48">
+      <c r="B13" s="7">
         <v>5</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="7">
         <v>5</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="7">
         <v>5</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="L13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="7">
         <v>5</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O13" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="P13" s="6" t="s">
+      <c r="P13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="V13" s="5">
+      <c r="V13" s="7">
         <v>5</v>
       </c>
-      <c r="W13" t="s">
+      <c r="W13" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="X13" s="6" t="s">
+      <c r="X13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="AH13" s="7">
+      <c r="AH13" s="10">
         <v>5</v>
       </c>
-      <c r="AI13" s="8" t="s">
+      <c r="AI13" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="AJ13" s="9" t="s">
+      <c r="AJ13" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="AL13" s="7">
+      <c r="AL13" s="10">
         <v>5</v>
       </c>
-      <c r="AM13" s="8" t="s">
+      <c r="AM13" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="AN13" s="9" t="s">
+      <c r="AN13" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B14" s="7">
+    <row r="14" spans="2:48">
+      <c r="B14" s="10">
         <v>6</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="10">
         <v>6</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="10">
         <v>6</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="K14" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="L14" s="9" t="s">
+      <c r="L14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N14" s="10">
         <v>6</v>
       </c>
-      <c r="O14" s="8" t="s">
+      <c r="O14" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="P14" s="9" t="s">
+      <c r="P14" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="V14" s="7">
+      <c r="V14" s="10">
         <v>6</v>
       </c>
-      <c r="W14" s="8" t="s">
+      <c r="W14" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="X14" s="9" t="s">
+      <c r="X14" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:48">
       <c r="B15">
         <v>7</v>
       </c>
@@ -1837,7 +1820,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:48">
       <c r="B16">
         <v>8</v>
       </c>
@@ -1875,7 +1858,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:16">
       <c r="B17">
         <v>9</v>
       </c>
@@ -1897,15 +1880,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="AP4:AR4"/>
-    <mergeCell ref="AP8:AR8"/>
-    <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AT8:AV8"/>
-    <mergeCell ref="AD8:AF8"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AH8:AJ8"/>
-    <mergeCell ref="AL4:AN4"/>
-    <mergeCell ref="AL8:AN8"/>
     <mergeCell ref="B1:AV2"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B8:D8"/>
@@ -1922,330 +1896,339 @@
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="Z8:AB8"/>
     <mergeCell ref="AD4:AF4"/>
+    <mergeCell ref="AD8:AF8"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AH8:AJ8"/>
+    <mergeCell ref="AL4:AN4"/>
+    <mergeCell ref="AL8:AN8"/>
+    <mergeCell ref="AP4:AR4"/>
+    <mergeCell ref="AP8:AR8"/>
+    <mergeCell ref="AT4:AV4"/>
+    <mergeCell ref="AT8:AV8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:X13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="1.7265625" customWidth="1"/>
-    <col min="2" max="2" width="4.26953125" customWidth="1"/>
-    <col min="3" max="3" width="17.7265625" customWidth="1"/>
-    <col min="4" max="4" width="7.7265625" customWidth="1"/>
-    <col min="5" max="5" width="1.7265625" customWidth="1"/>
-    <col min="6" max="6" width="4.26953125" customWidth="1"/>
-    <col min="7" max="7" width="18.7265625" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" customWidth="1"/>
-    <col min="9" max="9" width="1.7265625" customWidth="1"/>
-    <col min="10" max="10" width="4.26953125" customWidth="1"/>
-    <col min="11" max="11" width="19.7265625" customWidth="1"/>
-    <col min="12" max="12" width="5.7265625" customWidth="1"/>
-    <col min="13" max="13" width="1.7265625" customWidth="1"/>
-    <col min="14" max="14" width="4.26953125" customWidth="1"/>
-    <col min="15" max="15" width="15.7265625" customWidth="1"/>
-    <col min="16" max="16" width="5.7265625" customWidth="1"/>
-    <col min="17" max="17" width="1.7265625" customWidth="1"/>
-    <col min="18" max="18" width="4.26953125" customWidth="1"/>
-    <col min="19" max="19" width="17.7265625" customWidth="1"/>
-    <col min="20" max="20" width="9.7265625" customWidth="1"/>
-    <col min="21" max="21" width="1.7265625" customWidth="1"/>
-    <col min="22" max="22" width="4.26953125" customWidth="1"/>
-    <col min="23" max="23" width="18.7265625" customWidth="1"/>
-    <col min="24" max="24" width="5.7265625" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="1.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" customWidth="1"/>
+    <col min="13" max="13" width="1.7109375" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" customWidth="1"/>
+    <col min="17" max="17" width="1.7109375" customWidth="1"/>
+    <col min="18" max="18" width="4.28515625" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" customWidth="1"/>
+    <col min="21" max="21" width="1.7109375" customWidth="1"/>
+    <col min="22" max="22" width="4.28515625" customWidth="1"/>
+    <col min="23" max="23" width="18.7109375" customWidth="1"/>
+    <col min="24" max="24" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="2:24">
+      <c r="B1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-    </row>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-    </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B4" s="11" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+    </row>
+    <row r="2" spans="2:24">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+    </row>
+    <row r="4" spans="2:24">
+      <c r="B4" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="F4" s="11" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="F4" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="J4" s="11" t="s">
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="J4" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="N4" s="11" t="s">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="N4" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="R4" s="11" t="s">
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="R4" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="V4" s="11" t="s">
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="V4" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-    </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+    </row>
+    <row r="5" spans="2:24">
+      <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="G5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N5" s="1" t="s">
+      <c r="K5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="R5" s="1" t="s">
+      <c r="O5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="S5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="V5" s="1" t="s">
+      <c r="S5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="W5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B8" s="11" t="s">
+      <c r="W5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24">
+      <c r="B8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="F8" s="11" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="F8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="J8" s="11" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="J8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="N8" s="11" t="s">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="N8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="R8" s="11" t="s">
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="R8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="V8" s="11" t="s">
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="V8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-    </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+    </row>
+    <row r="9" spans="2:24">
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="2">
-        <v>1</v>
-      </c>
-      <c r="K9" s="3" t="s">
+      <c r="J9" s="4">
+        <v>1</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N9" s="2">
-        <v>1</v>
-      </c>
-      <c r="O9" s="3" t="s">
+      <c r="N9" s="4">
+        <v>1</v>
+      </c>
+      <c r="O9" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="P9" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="R9" s="2">
-        <v>1</v>
-      </c>
-      <c r="S9" s="3" t="s">
+      <c r="R9" s="4">
+        <v>1</v>
+      </c>
+      <c r="S9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="T9" s="4" t="s">
+      <c r="T9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="V9" s="2">
-        <v>1</v>
-      </c>
-      <c r="W9" s="3" t="s">
+      <c r="V9" s="4">
+        <v>1</v>
+      </c>
+      <c r="W9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="X9" s="4" t="s">
+      <c r="X9" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B10" s="7">
-        <v>2</v>
-      </c>
-      <c r="C10" s="8" t="s">
+    <row r="10" spans="2:24">
+      <c r="B10" s="10">
+        <v>2</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="7">
-        <v>2</v>
-      </c>
-      <c r="G10" s="8" t="s">
+      <c r="F10" s="10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="7">
-        <v>2</v>
-      </c>
-      <c r="K10" s="8" t="s">
+      <c r="J10" s="10">
+        <v>2</v>
+      </c>
+      <c r="K10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="L10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="N10" s="7">
-        <v>2</v>
-      </c>
-      <c r="O10" s="8" t="s">
+      <c r="N10" s="10">
+        <v>2</v>
+      </c>
+      <c r="O10" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="P10" s="9" t="s">
+      <c r="P10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="R10" s="7">
-        <v>2</v>
-      </c>
-      <c r="S10" s="8" t="s">
+      <c r="R10" s="10">
+        <v>2</v>
+      </c>
+      <c r="S10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="T10" s="9" t="s">
+      <c r="T10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="V10" s="7">
-        <v>2</v>
-      </c>
-      <c r="W10" s="8" t="s">
+      <c r="V10" s="10">
+        <v>2</v>
+      </c>
+      <c r="W10" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="X10" s="9" t="s">
+      <c r="X10" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:24">
       <c r="B11">
         <v>3</v>
       </c>
@@ -2283,7 +2266,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:24">
       <c r="F12">
         <v>4</v>
       </c>
@@ -2312,7 +2295,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:24">
       <c r="V13">
         <v>5</v>
       </c>
@@ -2344,275 +2327,275 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="1.7265625" customWidth="1"/>
-    <col min="2" max="2" width="4.26953125" customWidth="1"/>
-    <col min="3" max="3" width="16.7265625" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" customWidth="1"/>
-    <col min="5" max="5" width="1.7265625" customWidth="1"/>
-    <col min="6" max="6" width="4.26953125" customWidth="1"/>
-    <col min="7" max="7" width="17.7265625" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" customWidth="1"/>
-    <col min="9" max="9" width="1.7265625" customWidth="1"/>
-    <col min="10" max="10" width="4.26953125" customWidth="1"/>
-    <col min="11" max="11" width="14.7265625" customWidth="1"/>
-    <col min="12" max="12" width="17.7265625" customWidth="1"/>
-    <col min="13" max="13" width="1.7265625" customWidth="1"/>
-    <col min="14" max="14" width="4.26953125" customWidth="1"/>
-    <col min="15" max="15" width="14.7265625" customWidth="1"/>
-    <col min="16" max="16" width="17.7265625" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="1.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="13" max="13" width="1.7109375" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="2:16">
+      <c r="B1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-    </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B4" s="11" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="2:16">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="4" spans="2:16">
+      <c r="B4" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="F4" s="11" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="F4" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="J4" s="11" t="s">
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="J4" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="N4" s="11" t="s">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="N4" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="2:16">
+      <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="G5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N5" s="1" t="s">
+      <c r="K5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B8" s="11" t="s">
+      <c r="O5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16">
+      <c r="B8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="F8" s="11" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="F8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="J8" s="11" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="J8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="N8" s="11" t="s">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="N8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="2:16">
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="2">
-        <v>1</v>
-      </c>
-      <c r="K9" s="3" t="s">
+      <c r="J9" s="4">
+        <v>1</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="N9" s="2">
-        <v>1</v>
-      </c>
-      <c r="O9" s="3" t="s">
+      <c r="N9" s="4">
+        <v>1</v>
+      </c>
+      <c r="O9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="P9" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B10" s="5">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="10" spans="2:16">
+      <c r="B10" s="7">
+        <v>2</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="5">
-        <v>2</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="F10" s="7">
+        <v>2</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="7">
-        <v>2</v>
-      </c>
-      <c r="K10" s="8" t="s">
+      <c r="J10" s="10">
+        <v>2</v>
+      </c>
+      <c r="K10" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="L10" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="N10" s="5">
-        <v>2</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="N10" s="7">
+        <v>2</v>
+      </c>
+      <c r="O10" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="P10" s="6" t="s">
+      <c r="P10" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B11" s="5">
+    <row r="11" spans="2:16">
+      <c r="B11" s="7">
         <v>3</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="7">
         <v>3</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="10">
         <v>3</v>
       </c>
-      <c r="O11" s="8" t="s">
+      <c r="O11" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="P11" s="9" t="s">
+      <c r="P11" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B12" s="7">
+    <row r="12" spans="2:16">
+      <c r="B12" s="10">
         <v>4</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="10">
         <v>4</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:16">
       <c r="B13">
         <v>5</v>
       </c>
@@ -2632,7 +2615,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:16">
       <c r="B14">
         <v>6</v>
       </c>
@@ -2643,7 +2626,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:16">
       <c r="B15">
         <v>7</v>
       </c>
@@ -2671,237 +2654,237 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="1.7265625" customWidth="1"/>
-    <col min="2" max="2" width="4.26953125" customWidth="1"/>
-    <col min="3" max="3" width="30.7265625" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" customWidth="1"/>
-    <col min="5" max="5" width="1.7265625" customWidth="1"/>
-    <col min="6" max="6" width="4.26953125" customWidth="1"/>
-    <col min="7" max="7" width="30.7265625" customWidth="1"/>
-    <col min="8" max="8" width="17.7265625" customWidth="1"/>
-    <col min="9" max="9" width="1.7265625" customWidth="1"/>
-    <col min="10" max="10" width="4.26953125" customWidth="1"/>
-    <col min="11" max="11" width="30.7265625" customWidth="1"/>
-    <col min="12" max="12" width="5.7265625" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="1.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="2:12">
+      <c r="B1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B4" s="11" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="2:12">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="F4" s="11" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="F4" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="J4" s="11" t="s">
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="J4" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="G5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="11" t="s">
+      <c r="K5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="F8" s="11" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="F8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="J8" s="11" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="J8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="2">
-        <v>1</v>
-      </c>
-      <c r="K9" s="3" t="s">
+      <c r="J9" s="4">
+        <v>1</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B10" s="5">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="10" spans="2:12">
+      <c r="B10" s="7">
+        <v>2</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="5">
-        <v>2</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="F10" s="7">
+        <v>2</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="J10" s="5">
-        <v>2</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="J10" s="7">
+        <v>2</v>
+      </c>
+      <c r="K10" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B11" s="5">
+    <row r="11" spans="2:12">
+      <c r="B11" s="7">
         <v>3</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="10">
         <v>3</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="7">
         <v>3</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B12" s="5">
+    <row r="12" spans="2:12">
+      <c r="B12" s="7">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="10">
         <v>4</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="L12" s="9" t="s">
+      <c r="L12" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B13" s="7">
+    <row r="13" spans="2:12">
+      <c r="B13" s="10">
         <v>5</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12">
       <c r="B14">
         <v>6</v>
       </c>
@@ -2912,7 +2895,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:12">
       <c r="B15">
         <v>7</v>
       </c>
@@ -2923,7 +2906,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12">
       <c r="B16">
         <v>8</v>
       </c>

</xml_diff>